<commit_message>
script for merging in dry run with GA.  Other fun stuff.
</commit_message>
<xml_diff>
--- a/CSS2018/data/ClassInfo-Dev.xlsx
+++ b/CSS2018/data/ClassInfo-Dev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attendees" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Bob</t>
   </si>
@@ -192,13 +192,7 @@
     <t>IP</t>
   </si>
   <si>
-    <t>11.11.11.11</t>
-  </si>
-  <si>
     <t>Comment</t>
-  </si>
-  <si>
-    <t>bogus</t>
   </si>
   <si>
     <t>52.14.114.74</t>
@@ -562,12 +556,12 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -583,7 +577,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -591,7 +585,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -599,7 +593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -607,7 +601,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -615,7 +609,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -623,7 +617,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -631,7 +625,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -639,7 +633,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -647,7 +641,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -655,7 +649,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -663,7 +657,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -671,7 +665,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -679,7 +673,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -687,7 +681,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -695,7 +689,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -703,7 +697,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -711,7 +705,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -719,7 +713,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -727,7 +721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -735,7 +729,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -743,7 +737,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -751,7 +745,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -759,7 +753,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -767,7 +761,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -775,47 +769,47 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -827,18 +821,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -846,34 +840,23 @@
         <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
localhost home folder changed. Updates to all impacted slides. Dev of FN graph for merged data.
</commit_message>
<xml_diff>
--- a/CSS2018/data/ClassInfo-Dev.xlsx
+++ b/CSS2018/data/ClassInfo-Dev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attendees" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Server</t>
   </si>
@@ -57,29 +57,26 @@
     <t>18.219.116.80</t>
   </si>
   <si>
-    <t>no ping, no pull possible FROM this machine. Can pool INTO this machine</t>
-  </si>
-  <si>
     <t>Ping</t>
   </si>
   <si>
-    <t>to 18.218.251.17: Success</t>
-  </si>
-  <si>
-    <t>to 18.222.6.115: FAIL</t>
-  </si>
-  <si>
     <t>Core</t>
   </si>
   <si>
     <t>RAM (G)</t>
+  </si>
+  <si>
+    <t>For use by JU: 27-29-Feg</t>
+  </si>
+  <si>
+    <t>TW DEMO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,13 +90,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,12 +124,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,9 +452,9 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -454,18 +466,18 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.26953125" customWidth="1"/>
-    <col min="8" max="8" width="37.90625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="37.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,19 +485,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -503,34 +515,34 @@
         <v>Study1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>4</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E3" s="4" t="str">
         <f t="shared" ref="E3:E8" si="0">_xlfn.CONCAT("Study",A3)</f>
         <v>Study2</v>
       </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A8" si="1">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4">
@@ -543,14 +555,11 @@
         <f t="shared" si="0"/>
         <v>Study3</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -569,7 +578,7 @@
         <v>Study4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -588,7 +597,7 @@
         <v>Study5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -607,7 +616,7 @@
         <v>Study6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>7</v>

</xml_diff>